<commit_message>
updated models post var selection
</commit_message>
<xml_diff>
--- a/updated_scripts/data/glmm/selected_vars_glmm_abundance_obscot_clc2.xlsx
+++ b/updated_scripts/data/glmm/selected_vars_glmm_abundance_obscot_clc2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c73ee685cf225dcc/Desktop/uni/M2 stage/Cullicoides_data/updated_scripts/data/glmm/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c73ee685cf225dcc/Desktop/uni/M2 stage/Cullicoides_data/CIRAD/culicoides_ml/updated_scripts/data/glmm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{F223ABC1-DA54-45FE-B9B5-F67079476031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F2B5A59-53DB-489B-8842-1DC525DC8B80}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{F223ABC1-DA54-45FE-B9B5-F67079476031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2F0D2E0-96ED-4CBE-930F-EF8B68FEE738}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{F3649501-F1C5-4862-9529-397D11535757}"/>
+    <workbookView xWindow="6255" yWindow="-15600" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{F3649501-F1C5-4862-9529-397D11535757}"/>
   </bookViews>
   <sheets>
     <sheet name="glmm_abundance_obscot_clc2" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="107">
   <si>
     <t>term</t>
   </si>
@@ -333,6 +333,18 @@
   </si>
   <si>
     <t>maybe</t>
+  </si>
+  <si>
+    <t>FORCE ADDED</t>
+  </si>
+  <si>
+    <t>NDVI_0_6</t>
+  </si>
+  <si>
+    <t>SWV_0_0</t>
+  </si>
+  <si>
+    <t>not gonna include this one</t>
   </si>
 </sst>
 </file>
@@ -674,7 +686,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -861,6 +873,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -906,17 +927,35 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -928,25 +967,13 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1003,6 +1030,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2748,8 +2779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0931DFE-1A97-4492-B9A1-C69D87F0B65D}">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2758,38 +2789,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="L1" s="4" t="s">
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="L1" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="Q1" s="6" t="s">
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="Q1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="3" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C2" t="s">
@@ -2816,16 +2847,16 @@
       <c r="J2" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="Q2" s="5" t="s">
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="Q2" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="R2" s="5"/>
+      <c r="R2" s="14"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
@@ -2855,20 +2886,20 @@
       <c r="J3">
         <v>4.9481912970670401E-2</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="N3" s="8"/>
-      <c r="O3" s="9" t="s">
+      <c r="N3" s="16"/>
+      <c r="O3" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="Q3" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="R3" s="2" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2900,20 +2931,20 @@
       <c r="J4">
         <v>3.1650180861323297E-2</v>
       </c>
-      <c r="L4" s="10">
+      <c r="L4" s="5">
         <v>1</v>
       </c>
-      <c r="M4" s="11" t="s">
+      <c r="M4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="12"/>
-      <c r="O4" s="13" t="s">
+      <c r="N4" s="9"/>
+      <c r="O4" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="Q4" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="R4" s="2" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2945,20 +2976,20 @@
       <c r="J5">
         <v>2.3253849460902101E-2</v>
       </c>
-      <c r="L5" s="10">
+      <c r="L5" s="5">
         <v>2</v>
       </c>
-      <c r="M5" s="11" t="s">
+      <c r="M5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="N5" s="12"/>
-      <c r="O5" s="13" t="s">
+      <c r="N5" s="9"/>
+      <c r="O5" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="Q5" s="3" t="s">
+      <c r="Q5" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="R5" s="3" t="s">
+      <c r="R5" s="2" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2990,20 +3021,20 @@
       <c r="J6">
         <v>1.96492343862434E-2</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="5">
         <v>3</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="M6" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="N6" s="12"/>
-      <c r="O6" s="13" t="s">
+      <c r="N6" s="9"/>
+      <c r="O6" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="Q6" s="3" t="s">
+      <c r="Q6" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="R6" s="3" t="s">
+      <c r="R6" s="2" t="s">
         <v>87</v>
       </c>
     </row>
@@ -3035,20 +3066,20 @@
       <c r="J7">
         <v>3.9154523776961997E-3</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7" s="5">
         <v>5</v>
       </c>
-      <c r="M7" s="11" t="s">
+      <c r="M7" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="N7" s="12"/>
-      <c r="O7" s="13" t="s">
+      <c r="N7" s="9"/>
+      <c r="O7" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="Q7" s="3" t="s">
+      <c r="Q7" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="R7" s="3" t="s">
+      <c r="R7" s="2" t="s">
         <v>89</v>
       </c>
     </row>
@@ -3080,20 +3111,20 @@
       <c r="J8">
         <v>3.9154523776961997E-3</v>
       </c>
-      <c r="L8" s="10">
+      <c r="L8" s="5">
         <v>6</v>
       </c>
-      <c r="M8" s="11" t="s">
+      <c r="M8" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="N8" s="12"/>
-      <c r="O8" s="13" t="s">
+      <c r="N8" s="9"/>
+      <c r="O8" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="Q8" s="3" t="s">
+      <c r="Q8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="R8" s="3" t="s">
+      <c r="R8" s="2" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3125,20 +3156,20 @@
       <c r="J9">
         <v>4.9983783976910001E-2</v>
       </c>
-      <c r="L9" s="10">
+      <c r="L9" s="5">
         <v>7</v>
       </c>
-      <c r="M9" s="11" t="s">
+      <c r="M9" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="N9" s="12"/>
-      <c r="O9" s="14" t="s">
+      <c r="N9" s="9"/>
+      <c r="O9" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="Q9" s="3" t="s">
+      <c r="Q9" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="R9" s="3" t="s">
+      <c r="R9" s="2" t="s">
         <v>93</v>
       </c>
     </row>
@@ -3170,20 +3201,20 @@
       <c r="J10">
         <v>4.9983783976910001E-2</v>
       </c>
-      <c r="L10" s="10">
+      <c r="L10" s="5">
         <v>8</v>
       </c>
-      <c r="M10" s="11" t="s">
+      <c r="M10" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="N10" s="12"/>
-      <c r="O10" s="14" t="s">
+      <c r="N10" s="9"/>
+      <c r="O10" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="Q10" s="3" t="s">
+      <c r="Q10" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="R10" s="3" t="s">
+      <c r="R10" s="2" t="s">
         <v>95</v>
       </c>
     </row>
@@ -3215,16 +3246,20 @@
       <c r="J11">
         <v>3.9154523776961997E-3</v>
       </c>
-      <c r="L11" s="10">
+      <c r="L11" s="5">
         <v>9</v>
       </c>
-      <c r="M11" s="11" t="s">
+      <c r="M11" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="N11" s="12"/>
-      <c r="O11" s="14" t="s">
+      <c r="N11" s="9"/>
+      <c r="O11" s="7" t="s">
         <v>70</v>
       </c>
+      <c r="Q11" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="R11" s="11"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
@@ -3254,18 +3289,24 @@
       <c r="J12">
         <v>4.9689054929162103E-4</v>
       </c>
-      <c r="L12" s="10">
+      <c r="L12" s="5">
         <v>10</v>
       </c>
-      <c r="M12" s="16" t="s">
+      <c r="M12" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="N12" s="17"/>
-      <c r="O12" s="14" t="s">
+      <c r="N12" s="18"/>
+      <c r="O12" s="7" t="s">
         <v>70</v>
       </c>
       <c r="P12" t="s">
         <v>96</v>
+      </c>
+      <c r="Q12" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="R12" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
@@ -3296,15 +3337,18 @@
       <c r="J13">
         <v>8.5465508467139004E-3</v>
       </c>
-      <c r="L13" s="10">
+      <c r="L13" s="5">
         <v>11</v>
       </c>
-      <c r="M13" s="16" t="s">
+      <c r="M13" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="N13" s="17"/>
-      <c r="O13" s="14" t="s">
+      <c r="N13" s="18"/>
+      <c r="O13" s="7" t="s">
         <v>70</v>
+      </c>
+      <c r="R13" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
@@ -3335,14 +3379,14 @@
       <c r="J14">
         <v>1.11318949052481E-2</v>
       </c>
-      <c r="L14" s="10">
+      <c r="L14" s="5">
         <v>12</v>
       </c>
-      <c r="M14" s="11" t="s">
+      <c r="M14" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="N14" s="12"/>
-      <c r="O14" s="14" t="s">
+      <c r="N14" s="9"/>
+      <c r="O14" s="7" t="s">
         <v>70</v>
       </c>
       <c r="P14" t="s">
@@ -3377,14 +3421,14 @@
       <c r="J15">
         <v>1.0677522109865799E-3</v>
       </c>
-      <c r="L15" s="10">
+      <c r="L15" s="5">
         <v>13</v>
       </c>
-      <c r="M15" s="11" t="s">
+      <c r="M15" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="N15" s="12"/>
-      <c r="O15" s="14" t="s">
+      <c r="N15" s="9"/>
+      <c r="O15" s="7" t="s">
         <v>70</v>
       </c>
       <c r="P15" t="s">
@@ -3419,14 +3463,14 @@
       <c r="J16">
         <v>1.3814341415215901E-2</v>
       </c>
-      <c r="L16" s="10">
+      <c r="L16" s="5">
         <v>14</v>
       </c>
-      <c r="M16" s="16" t="s">
+      <c r="M16" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="N16" s="17"/>
-      <c r="O16" s="14" t="s">
+      <c r="N16" s="18"/>
+      <c r="O16" s="7" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3458,14 +3502,14 @@
       <c r="J17">
         <v>1.3814341415215901E-2</v>
       </c>
-      <c r="L17" s="10">
+      <c r="L17" s="5">
         <v>15</v>
       </c>
-      <c r="M17" s="16" t="s">
+      <c r="M17" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="N17" s="17"/>
-      <c r="O17" s="14" t="s">
+      <c r="N17" s="18"/>
+      <c r="O17" s="7" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3497,14 +3541,14 @@
       <c r="J18">
         <v>5.48231549795257E-4</v>
       </c>
-      <c r="L18" s="10">
+      <c r="L18" s="5">
         <v>16</v>
       </c>
-      <c r="M18" s="11" t="s">
+      <c r="M18" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="N18" s="12"/>
-      <c r="O18" s="14" t="s">
+      <c r="N18" s="9"/>
+      <c r="O18" s="7" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3536,12 +3580,12 @@
       <c r="J19">
         <v>8.3008790548555599E-3</v>
       </c>
-      <c r="L19" s="10">
+      <c r="L19" s="5">
         <v>17</v>
       </c>
-      <c r="M19" s="11"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="15"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="2"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
@@ -3776,7 +3820,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="23">
     <mergeCell ref="M19:N19"/>
     <mergeCell ref="M14:N14"/>
     <mergeCell ref="M16:N16"/>
@@ -3793,12 +3837,13 @@
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="Q11:R11"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:J1"/>
     <mergeCell ref="L1:O1"/>
     <mergeCell ref="L2:O2"/>
     <mergeCell ref="M3:N3"/>
-    <mergeCell ref="M4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>